<commit_message>
added two new old rules
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lusine/Documents/Masterarbeit/Code/MA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF27F3F2-8709-324E-8079-33B49AF0E9DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52881F5-6039-F148-9F5E-4CC06E5C6983}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2480" yWindow="-18960" windowWidth="35760" windowHeight="18120" xr2:uid="{CBBA58C6-C4C8-8F40-AC78-68ADD622581E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{CBBA58C6-C4C8-8F40-AC78-68ADD622581E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="175">
   <si>
     <t>GCContent</t>
   </si>
@@ -544,6 +544,12 @@
   </si>
   <si>
     <t>Skript/ Daten von CADD mit anderem Window</t>
+  </si>
+  <si>
+    <t>https://hgdownload.soe.ucsc.edu/goldenPath/hg38/phyloP30way/hg38.30way.phyloP/</t>
+  </si>
+  <si>
+    <t>https://hgdownload.soe.ucsc.edu/goldenPath/hg38/phastCons30way/hg38.30way.phastCons/</t>
   </si>
 </sst>
 </file>
@@ -976,7 +982,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="150" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1197,7 +1203,7 @@
         <v>146</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>151</v>
@@ -1271,7 +1277,7 @@
         <v>145</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>145</v>
+        <v>174</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>151</v>
@@ -1309,7 +1315,7 @@
         <v>145</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>145</v>
+        <v>174</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>151</v>
@@ -1334,7 +1340,7 @@
       <c r="F10" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="13" t="s">
         <v>25</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -1376,7 +1382,7 @@
         <v>145</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>145</v>
+        <v>174</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>151</v>
@@ -1915,26 +1921,23 @@
     <hyperlink ref="H7" r:id="rId13" xr:uid="{04F57986-A16C-2643-94A8-1BDAD35F054B}"/>
     <hyperlink ref="H8" r:id="rId14" xr:uid="{2107AEAD-FBFF-E747-8CC1-7C1EA72BE313}"/>
     <hyperlink ref="K2" r:id="rId15" xr:uid="{045EBF81-6802-2746-84B0-D9B73A72F658}"/>
-    <hyperlink ref="K6" r:id="rId16" xr:uid="{FC146EE3-9D7C-4248-BD84-CB1F71E8C330}"/>
-    <hyperlink ref="N6" r:id="rId17" display="https://hgdownload.soe.ucsc.edu/goldenPath/hg38/phyloP30way/hg38.phyloP30way.bw" xr:uid="{D6F228D1-D7BF-F743-9C2A-11D2D059B158}"/>
-    <hyperlink ref="K7" r:id="rId18" xr:uid="{42FE9152-DEED-294C-B12E-966D3808CE99}"/>
-    <hyperlink ref="K8" r:id="rId19" xr:uid="{666B8F5C-132A-4A4C-A93E-B2F2C9F3B677}"/>
-    <hyperlink ref="K9" r:id="rId20" xr:uid="{D5A4776F-13DD-7343-A2A4-52BAF40B249C}"/>
-    <hyperlink ref="K10" r:id="rId21" xr:uid="{4A992BCD-91C0-EA4B-BA50-F0612D2AED61}"/>
-    <hyperlink ref="K11" r:id="rId22" xr:uid="{BE5FFC2A-01DD-404E-85F0-143CC9688CC3}"/>
-    <hyperlink ref="J17" r:id="rId23" xr:uid="{BCDFC0C2-446F-1745-84BF-0DF42B2F64CA}"/>
-    <hyperlink ref="J18" r:id="rId24" xr:uid="{F4F6CB96-FBC5-B44E-A65F-E691D354A120}"/>
-    <hyperlink ref="J14" r:id="rId25" xr:uid="{B32340A8-8FDD-FF43-B0F3-3D7ADE52C105}"/>
-    <hyperlink ref="J2" r:id="rId26" xr:uid="{D4CFA2A8-DE3E-4644-9B8F-7DA8A0385204}"/>
-    <hyperlink ref="J6" r:id="rId27" xr:uid="{DC2D198F-7697-4746-8534-602294D25B6A}"/>
-    <hyperlink ref="J7" r:id="rId28" xr:uid="{491B1A79-0E93-344E-B205-B0112E734A57}"/>
-    <hyperlink ref="J8" r:id="rId29" xr:uid="{CED81CB1-EEC4-FB42-8BE9-3A658CDEA89B}"/>
-    <hyperlink ref="J9" r:id="rId30" xr:uid="{194A2BA7-6B8B-6141-B96A-3CB179415622}"/>
-    <hyperlink ref="J10" r:id="rId31" xr:uid="{705C05DB-2805-6B4E-949A-4013A707E061}"/>
-    <hyperlink ref="J11" r:id="rId32" xr:uid="{98CAA680-4EE4-9549-ABFB-4673443BF3E5}"/>
-    <hyperlink ref="J12" r:id="rId33" xr:uid="{F1C84409-E11F-2A42-8685-7DA65C99B464}"/>
-    <hyperlink ref="K26" r:id="rId34" xr:uid="{E5A01AF7-2007-2247-A6A3-B083CF779CBC}"/>
-    <hyperlink ref="H12" r:id="rId35" xr:uid="{4543D07C-1E4B-004F-BFCF-518D1C872884}"/>
+    <hyperlink ref="N6" r:id="rId16" display="https://hgdownload.soe.ucsc.edu/goldenPath/hg38/phyloP30way/hg38.phyloP30way.bw" xr:uid="{D6F228D1-D7BF-F743-9C2A-11D2D059B158}"/>
+    <hyperlink ref="K7" r:id="rId17" xr:uid="{42FE9152-DEED-294C-B12E-966D3808CE99}"/>
+    <hyperlink ref="K10" r:id="rId18" xr:uid="{4A992BCD-91C0-EA4B-BA50-F0612D2AED61}"/>
+    <hyperlink ref="J17" r:id="rId19" xr:uid="{BCDFC0C2-446F-1745-84BF-0DF42B2F64CA}"/>
+    <hyperlink ref="J18" r:id="rId20" xr:uid="{F4F6CB96-FBC5-B44E-A65F-E691D354A120}"/>
+    <hyperlink ref="J14" r:id="rId21" xr:uid="{B32340A8-8FDD-FF43-B0F3-3D7ADE52C105}"/>
+    <hyperlink ref="J2" r:id="rId22" xr:uid="{D4CFA2A8-DE3E-4644-9B8F-7DA8A0385204}"/>
+    <hyperlink ref="J6" r:id="rId23" xr:uid="{DC2D198F-7697-4746-8534-602294D25B6A}"/>
+    <hyperlink ref="J7" r:id="rId24" xr:uid="{491B1A79-0E93-344E-B205-B0112E734A57}"/>
+    <hyperlink ref="J8" r:id="rId25" xr:uid="{CED81CB1-EEC4-FB42-8BE9-3A658CDEA89B}"/>
+    <hyperlink ref="J9" r:id="rId26" xr:uid="{194A2BA7-6B8B-6141-B96A-3CB179415622}"/>
+    <hyperlink ref="J10" r:id="rId27" xr:uid="{705C05DB-2805-6B4E-949A-4013A707E061}"/>
+    <hyperlink ref="J11" r:id="rId28" xr:uid="{98CAA680-4EE4-9549-ABFB-4673443BF3E5}"/>
+    <hyperlink ref="J12" r:id="rId29" xr:uid="{F1C84409-E11F-2A42-8685-7DA65C99B464}"/>
+    <hyperlink ref="K26" r:id="rId30" xr:uid="{E5A01AF7-2007-2247-A6A3-B083CF779CBC}"/>
+    <hyperlink ref="H12" r:id="rId31" xr:uid="{4543D07C-1E4B-004F-BFCF-518D1C872884}"/>
+    <hyperlink ref="H10" r:id="rId32" xr:uid="{C3CF0E15-8219-2546-A4BA-3A4CAAEBF211}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>